<commit_message>
Round,Enemy Data Excel To Json
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\Storm The House\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3170B16C-A792-4034-9CC3-DC0867BE034D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AA733D-9310-4011-88C2-0327F7CB40B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-28080" yWindow="6345" windowWidth="16290" windowHeight="12105" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
+    <sheet name="Enemy" sheetId="2" r:id="rId2"/>
+    <sheet name="Round" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="104">
   <si>
     <t>AMMO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -310,6 +312,78 @@
   </si>
   <si>
     <t>cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWORD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARATROOPER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOMBCAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TANK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HELICOPTER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROBOT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROUND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPEED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATTACKDELAY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATTACKRANGE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MONEY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLAMETHROWER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VALUE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -676,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D884F8-0FD5-40CA-AEA1-09465B4050E8}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1221,4 +1295,1593 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CFB178-60C6-42BA-9A7C-03EB8A68EE9C}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0.25</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8">
+        <v>150</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10">
+        <v>270</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E089036-B500-4741-BD5D-60098B606228}">
+  <dimension ref="A1:M41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="str">
+        <f>Enemy!A2</f>
+        <v>SWORD</v>
+      </c>
+      <c r="C1" t="str">
+        <f>Enemy!A3</f>
+        <v>GUN</v>
+      </c>
+      <c r="D1" t="str">
+        <f>Enemy!A4</f>
+        <v>CAR</v>
+      </c>
+      <c r="E1" t="str">
+        <f>Enemy!A5</f>
+        <v>PARATROOPER</v>
+      </c>
+      <c r="F1" t="str">
+        <f>Enemy!A6</f>
+        <v>BOMBCAR</v>
+      </c>
+      <c r="G1" t="str">
+        <f>Enemy!A7</f>
+        <v>FLAMETHROWER</v>
+      </c>
+      <c r="H1" t="str">
+        <f>Enemy!A8</f>
+        <v>TANK</v>
+      </c>
+      <c r="I1" t="str">
+        <f>Enemy!A9</f>
+        <v>HELICOPTER</v>
+      </c>
+      <c r="J1" t="str">
+        <f>Enemy!A10</f>
+        <v>ROBOT</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <f>B2*20+C2*50+D2*100+E2*60+F2*150+G2*130+H2*180+I2*100+J2*1000</f>
+        <v>1000</v>
+      </c>
+      <c r="L2">
+        <v>900</v>
+      </c>
+      <c r="M2">
+        <f>L2-K2</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K39" si="0">B3*20+C3*50+D3*100+E3*60+F3*150+G3*130+H3*180+I3*100+J3*1000</f>
+        <v>1500</v>
+      </c>
+      <c r="L3">
+        <v>1400</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M42" si="1">L3-K3</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="L4">
+        <v>1900</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>125</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="L5">
+        <v>2400</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="L6">
+        <v>2900</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>175</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>3800</v>
+      </c>
+      <c r="L7">
+        <v>3600</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>4600</v>
+      </c>
+      <c r="L8">
+        <v>4300</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>225</v>
+      </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>5400</v>
+      </c>
+      <c r="L9">
+        <v>5000</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>-400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>250</v>
+      </c>
+      <c r="C10">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>6700</v>
+      </c>
+      <c r="L10">
+        <v>6500</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>275</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="L11">
+        <v>8000</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>300</v>
+      </c>
+      <c r="C12">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>9300</v>
+      </c>
+      <c r="L12">
+        <v>9500</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>325</v>
+      </c>
+      <c r="C13">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>10600</v>
+      </c>
+      <c r="L13">
+        <v>11000</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>350</v>
+      </c>
+      <c r="C14">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>11900</v>
+      </c>
+      <c r="L14">
+        <v>12500</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>375</v>
+      </c>
+      <c r="C15">
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>13200</v>
+      </c>
+      <c r="L15">
+        <v>14000</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>400</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>35</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>14500</v>
+      </c>
+      <c r="L16">
+        <v>15500</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>425</v>
+      </c>
+      <c r="C17">
+        <v>66</v>
+      </c>
+      <c r="D17">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>16700</v>
+      </c>
+      <c r="L17">
+        <v>17000</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>450</v>
+      </c>
+      <c r="C18">
+        <v>72</v>
+      </c>
+      <c r="D18">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>18300</v>
+      </c>
+      <c r="L18">
+        <v>20000</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>475</v>
+      </c>
+      <c r="C19">
+        <v>78</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>19900</v>
+      </c>
+      <c r="L19">
+        <v>21500</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>500</v>
+      </c>
+      <c r="C20">
+        <v>84</v>
+      </c>
+      <c r="D20">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>22800</v>
+      </c>
+      <c r="L20">
+        <v>25500</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>525</v>
+      </c>
+      <c r="C21">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>24660</v>
+      </c>
+      <c r="L21">
+        <v>27000</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>550</v>
+      </c>
+      <c r="C22">
+        <v>96</v>
+      </c>
+      <c r="D22">
+        <v>65</v>
+      </c>
+      <c r="E22">
+        <v>35</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>14</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>26670</v>
+      </c>
+      <c r="L22">
+        <v>28500</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>575</v>
+      </c>
+      <c r="C23">
+        <v>102</v>
+      </c>
+      <c r="D23">
+        <v>70</v>
+      </c>
+      <c r="E23">
+        <v>40</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>16</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>28530</v>
+      </c>
+      <c r="L23">
+        <v>30000</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>600</v>
+      </c>
+      <c r="C24">
+        <v>108</v>
+      </c>
+      <c r="D24">
+        <v>75</v>
+      </c>
+      <c r="E24">
+        <v>45</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>18</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>30390</v>
+      </c>
+      <c r="L24">
+        <v>31500</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>625</v>
+      </c>
+      <c r="C25">
+        <v>114</v>
+      </c>
+      <c r="D25">
+        <v>80</v>
+      </c>
+      <c r="E25">
+        <v>50</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>20</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>32250</v>
+      </c>
+      <c r="L25">
+        <v>33000</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>650</v>
+      </c>
+      <c r="C26">
+        <v>120</v>
+      </c>
+      <c r="D26">
+        <v>85</v>
+      </c>
+      <c r="E26">
+        <v>55</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>22</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>34110</v>
+      </c>
+      <c r="L26">
+        <v>34500</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>675</v>
+      </c>
+      <c r="C27">
+        <v>126</v>
+      </c>
+      <c r="D27">
+        <v>90</v>
+      </c>
+      <c r="E27">
+        <v>60</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>24</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>37920</v>
+      </c>
+      <c r="L27">
+        <v>36000</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>-1920</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>700</v>
+      </c>
+      <c r="C28">
+        <v>132</v>
+      </c>
+      <c r="D28">
+        <v>95</v>
+      </c>
+      <c r="E28">
+        <v>65</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>26</v>
+      </c>
+      <c r="H28">
+        <v>12</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>40140</v>
+      </c>
+      <c r="L28">
+        <v>38500</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>-1640</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>725</v>
+      </c>
+      <c r="C29">
+        <v>138</v>
+      </c>
+      <c r="D29">
+        <v>100</v>
+      </c>
+      <c r="E29">
+        <v>70</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>14</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>42360</v>
+      </c>
+      <c r="L29">
+        <v>41000</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>-1360</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>750</v>
+      </c>
+      <c r="C30">
+        <v>144</v>
+      </c>
+      <c r="D30">
+        <v>105</v>
+      </c>
+      <c r="E30">
+        <v>75</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>30</v>
+      </c>
+      <c r="H30">
+        <v>16</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>45580</v>
+      </c>
+      <c r="L30">
+        <v>44500</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>-1080</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>775</v>
+      </c>
+      <c r="C31">
+        <v>150</v>
+      </c>
+      <c r="D31">
+        <v>110</v>
+      </c>
+      <c r="E31">
+        <v>80</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>32</v>
+      </c>
+      <c r="H31">
+        <v>18</v>
+      </c>
+      <c r="I31">
+        <v>12</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>48000</v>
+      </c>
+      <c r="L31">
+        <v>46000</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>800</v>
+      </c>
+      <c r="C32">
+        <v>156</v>
+      </c>
+      <c r="D32">
+        <v>115</v>
+      </c>
+      <c r="E32">
+        <v>85</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>34</v>
+      </c>
+      <c r="H32">
+        <v>20</v>
+      </c>
+      <c r="I32">
+        <v>14</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>50570</v>
+      </c>
+      <c r="L32">
+        <v>50000</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>-570</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>825</v>
+      </c>
+      <c r="C33">
+        <v>162</v>
+      </c>
+      <c r="D33">
+        <v>120</v>
+      </c>
+      <c r="E33">
+        <v>90</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>36</v>
+      </c>
+      <c r="H33">
+        <v>22</v>
+      </c>
+      <c r="I33">
+        <v>16</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>52990</v>
+      </c>
+      <c r="L33">
+        <v>51500</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>-1490</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>850</v>
+      </c>
+      <c r="C34">
+        <v>168</v>
+      </c>
+      <c r="D34">
+        <v>125</v>
+      </c>
+      <c r="E34">
+        <v>95</v>
+      </c>
+      <c r="F34">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>38</v>
+      </c>
+      <c r="H34">
+        <v>24</v>
+      </c>
+      <c r="I34">
+        <v>18</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>55410</v>
+      </c>
+      <c r="L34">
+        <v>57500</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>875</v>
+      </c>
+      <c r="C35">
+        <v>174</v>
+      </c>
+      <c r="D35">
+        <v>130</v>
+      </c>
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>40</v>
+      </c>
+      <c r="H35">
+        <v>26</v>
+      </c>
+      <c r="I35">
+        <v>20</v>
+      </c>
+      <c r="J35">
+        <v>5</v>
+      </c>
+      <c r="K35">
+        <f>B35*20+C35*50+D35*100+E35*60+F35*150+G35*130+H35*180+I35*100+J35*1000</f>
+        <v>62830</v>
+      </c>
+      <c r="L35">
+        <v>59000</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>-3830</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>900</v>
+      </c>
+      <c r="C36">
+        <v>180</v>
+      </c>
+      <c r="D36">
+        <v>135</v>
+      </c>
+      <c r="E36">
+        <v>105</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
+        <v>42</v>
+      </c>
+      <c r="H36">
+        <v>28</v>
+      </c>
+      <c r="I36">
+        <v>22</v>
+      </c>
+      <c r="J36">
+        <v>8</v>
+      </c>
+      <c r="K36">
+        <f>B36*20+C36*50+D36*100+E36*60+F36*150+G36*130+H36*180+I36*100+J36*1000</f>
+        <v>68250</v>
+      </c>
+      <c r="L36">
+        <v>68000</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>925</v>
+      </c>
+      <c r="C37">
+        <v>186</v>
+      </c>
+      <c r="D37">
+        <v>140</v>
+      </c>
+      <c r="E37">
+        <v>110</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>44</v>
+      </c>
+      <c r="H37">
+        <v>30</v>
+      </c>
+      <c r="I37">
+        <v>24</v>
+      </c>
+      <c r="J37">
+        <v>11</v>
+      </c>
+      <c r="K37">
+        <f>B37*20+C37*50+D37*100+E37*60+F37*150+G37*130+H37*180+I37*100+J37*1000</f>
+        <v>73820</v>
+      </c>
+      <c r="L37">
+        <v>68000</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="1"/>
+        <v>-5820</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>950</v>
+      </c>
+      <c r="C38">
+        <v>192</v>
+      </c>
+      <c r="D38">
+        <v>145</v>
+      </c>
+      <c r="E38">
+        <v>115</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>46</v>
+      </c>
+      <c r="H38">
+        <v>32</v>
+      </c>
+      <c r="I38">
+        <v>26</v>
+      </c>
+      <c r="J38">
+        <v>14</v>
+      </c>
+      <c r="K38">
+        <f>B38*20+C38*50+D38*100+E38*60+F38*150+G38*130+H38*180+I38*100+J38*1000</f>
+        <v>79240</v>
+      </c>
+      <c r="L38">
+        <v>80000</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="1"/>
+        <v>760</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>975</v>
+      </c>
+      <c r="C39">
+        <v>198</v>
+      </c>
+      <c r="D39">
+        <v>150</v>
+      </c>
+      <c r="E39">
+        <v>120</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>48</v>
+      </c>
+      <c r="H39">
+        <v>34</v>
+      </c>
+      <c r="I39">
+        <v>28</v>
+      </c>
+      <c r="J39">
+        <v>17</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>84660</v>
+      </c>
+      <c r="L39">
+        <v>82000</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>-2660</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1000</v>
+      </c>
+      <c r="C40">
+        <v>204</v>
+      </c>
+      <c r="D40">
+        <v>155</v>
+      </c>
+      <c r="E40">
+        <v>125</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
+      </c>
+      <c r="G40">
+        <v>50</v>
+      </c>
+      <c r="H40">
+        <v>36</v>
+      </c>
+      <c r="I40">
+        <v>30</v>
+      </c>
+      <c r="J40">
+        <v>20</v>
+      </c>
+      <c r="K40">
+        <f>B40*20+C40*50+D40*100+E40*60+F40*150+G40*130+H40*180+I40*100+J40*1000</f>
+        <v>90080</v>
+      </c>
+      <c r="L40">
+        <v>95000</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="1"/>
+        <v>4920</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1025</v>
+      </c>
+      <c r="C41">
+        <v>210</v>
+      </c>
+      <c r="D41">
+        <v>160</v>
+      </c>
+      <c r="E41">
+        <v>130</v>
+      </c>
+      <c r="F41">
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <v>52</v>
+      </c>
+      <c r="H41">
+        <v>38</v>
+      </c>
+      <c r="I41">
+        <v>32</v>
+      </c>
+      <c r="J41">
+        <v>23</v>
+      </c>
+      <c r="K41">
+        <f>B41*20+C41*50+D41*100+E41*60+F41*150+G41*130+H41*180+I41*100+J41*1000</f>
+        <v>95500</v>
+      </c>
+      <c r="L41">
+        <v>92000</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="1"/>
+        <v>-3500</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Item Image & Icon
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\Storm The House\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AA733D-9310-4011-88C2-0327F7CB40B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8919FF49-F208-400E-8644-5896B4069FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28080" yWindow="6345" windowWidth="16290" windowHeight="12105" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>AMMO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,9 +87,6 @@
     <t>CAHINSAW</t>
   </si>
   <si>
-    <t>GRANADE LAUNCHER</t>
-  </si>
-  <si>
     <t>SPACE LASER</t>
   </si>
   <si>
@@ -384,6 +381,64 @@
   </si>
   <si>
     <t>VALUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A drive-by favorite, the uzi is an affordable, fuuly automatic solution to all your semi-automatic problems.</t>
+  </si>
+  <si>
+    <t>Rednecks and zombie slayers agree, shotguns are always a good decision. Don’t forget… shop smart, shop S-mart.</t>
+  </si>
+  <si>
+    <t>You’re standard automatic rifle. Accurate and powerful. A step above that cute lil’ uzi.</t>
+  </si>
+  <si>
+    <t>A ballsier, automatic version of the combat shotgun. For when you really need to call down the rain.</t>
+  </si>
+  <si>
+    <t>Perfect for getting rid of termites, hilarious WWII reenactments with friends, or even when your son’s little league game runs long. The flame thrower. Don’t leave home without it.</t>
+  </si>
+  <si>
+    <t>When Sylvester stalone needs to cut down row after row of Vietcong soldiers and emerge with nothing but stainless steel abs and the sweat on his brow, you better believe he brings his machine gun.</t>
+  </si>
+  <si>
+    <t>“There’s a chainsaw? Sweet!” - You</t>
+  </si>
+  <si>
+    <t>Perfect for launching grenades.</t>
+  </si>
+  <si>
+    <t>This baby focuses a satellite mounted laser at your feeble enemies and promptly deatomizes them.</t>
+  </si>
+  <si>
+    <t>Handheld tele-geo-dynamics manipulating oscillator generator capable of knocking down troops and damaging vehicles.</t>
+  </si>
+  <si>
+    <t>A gun so big it overlaps the buy button.</t>
+  </si>
+  <si>
+    <t>This giant fan has a slowing effect that will stop those puny swordmen right in their trakcs. LOL!</t>
+  </si>
+  <si>
+    <t>This beastbox initiates minor tremors causing foot soldiers to fall over and armored units to take damage.</t>
+  </si>
+  <si>
+    <t>Known by scientists as the “Magnificant Wallopping Van De Graaff Machine”, the tesla tower delivers lethally concentrated bolts of electricity at a short range.</t>
+  </si>
+  <si>
+    <t>Fires heat seeking missiles that damage all units within it’s blast radius.</t>
+  </si>
+  <si>
+    <t>The M6 Laser Tower fires a very powerful blast of energy at the toughest enemy on the screen.</t>
+  </si>
+  <si>
+    <t>Flamer Joe likes to set people on fire.</t>
+  </si>
+  <si>
+    <t>Generates a protective shield that cuts all damage taken by a percentage.</t>
+  </si>
+  <si>
+    <t>GRENADE LAUNCHER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -750,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D884F8-0FD5-40CA-AEA1-09465B4050E8}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -764,19 +819,19 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -788,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -800,16 +855,16 @@
         <v>5</v>
       </c>
       <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -823,19 +878,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -849,19 +904,19 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E3">
         <v>300</v>
       </c>
       <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>34</v>
-      </c>
-      <c r="H3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -875,19 +930,19 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E4">
         <v>2000</v>
       </c>
       <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>37</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -901,19 +956,19 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="E5">
         <v>5000</v>
       </c>
       <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
         <v>39</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -927,19 +982,19 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E6">
         <v>4000</v>
       </c>
       <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
         <v>42</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -953,19 +1008,19 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="E7">
         <v>7500</v>
       </c>
       <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>46</v>
-      </c>
-      <c r="K7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -979,19 +1034,19 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="E8">
         <v>11000</v>
       </c>
       <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
         <v>48</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>49</v>
-      </c>
-      <c r="H8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1005,19 +1060,19 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="E9">
         <v>5000</v>
       </c>
       <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
         <v>51</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>52</v>
-      </c>
-      <c r="J9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1025,25 +1080,25 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="E10">
         <v>10000</v>
       </c>
       <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
         <v>54</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>55</v>
-      </c>
-      <c r="J10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1051,25 +1106,25 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="E11">
         <v>20000</v>
       </c>
       <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" t="s">
         <v>57</v>
       </c>
-      <c r="H11" t="s">
+      <c r="K11" t="s">
         <v>58</v>
-      </c>
-      <c r="K11" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1077,25 +1132,25 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="E12">
         <v>7000</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" t="s">
         <v>60</v>
-      </c>
-      <c r="J12" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1103,25 +1158,25 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="E13">
         <v>30000</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" t="s">
         <v>62</v>
-      </c>
-      <c r="H13" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1129,22 +1184,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="E15">
         <v>2000</v>
       </c>
       <c r="K15" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" t="s">
         <v>64</v>
-      </c>
-      <c r="O15" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -1152,19 +1207,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="E16">
         <v>2000</v>
       </c>
       <c r="I16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P16" t="b">
         <v>1</v>
@@ -1175,25 +1230,25 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="E17">
         <v>4000</v>
       </c>
       <c r="I17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" t="s">
         <v>67</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>68</v>
-      </c>
-      <c r="K17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1201,25 +1256,25 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="E18">
         <v>6000</v>
       </c>
       <c r="I18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" t="s">
         <v>70</v>
       </c>
-      <c r="J18" t="s">
+      <c r="M18" t="s">
         <v>71</v>
-      </c>
-      <c r="M18" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1227,22 +1282,22 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="E19">
         <v>8000</v>
       </c>
       <c r="I19" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" t="s">
         <v>73</v>
-      </c>
-      <c r="J19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1250,25 +1305,25 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="E20">
         <v>5000</v>
       </c>
       <c r="I20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" t="s">
         <v>75</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>76</v>
-      </c>
-      <c r="K20" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1276,19 +1331,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="E21">
         <v>3000</v>
       </c>
       <c r="N21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1309,30 +1364,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>96</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>97</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>99</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>100</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1355,7 +1410,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1378,7 +1433,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -1401,7 +1456,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -1424,7 +1479,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1447,7 +1502,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7">
         <v>35</v>
@@ -1470,7 +1525,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8">
         <v>150</v>
@@ -1493,7 +1548,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -1516,7 +1571,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10">
         <v>270</v>
@@ -1547,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E089036-B500-4741-BD5D-60098B606228}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -1559,7 +1614,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" t="str">
         <f>Enemy!A2</f>
@@ -1598,7 +1653,7 @@
         <v>ROBOT</v>
       </c>
       <c r="K1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1635,7 +1690,7 @@
         <v>1400</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M42" si="1">L3-K3</f>
+        <f t="shared" ref="M3:M41" si="1">L3-K3</f>
         <v>-100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust Enemy Attack Delay
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\Storm The House\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9822F162-0C87-47BA-B8D2-9262572E6E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8883B417-F38E-45BE-83CD-40868622F718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27450" yWindow="5250" windowWidth="26640" windowHeight="14940" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-19575" yWindow="6195" windowWidth="16710" windowHeight="10965" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="168">
   <si>
     <t>AMMO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -630,6 +630,10 @@
   </si>
   <si>
     <t>8;0;8;0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100;0;100;0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1059,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D884F8-0FD5-40CA-AEA1-09465B4050E8}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1071,7 +1075,7 @@
     <col min="4" max="4" width="9.5" customWidth="1"/>
     <col min="5" max="5" width="6.5" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="6.375" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="15" width="15.75" customWidth="1"/>
     <col min="16" max="16" width="16.125" customWidth="1"/>
   </cols>
@@ -1341,6 +1345,9 @@
       <c r="G7" t="s">
         <v>40</v>
       </c>
+      <c r="H7" t="s">
+        <v>167</v>
+      </c>
       <c r="I7" t="s">
         <v>41</v>
       </c>
@@ -1417,6 +1424,9 @@
       <c r="G9" t="s">
         <v>45</v>
       </c>
+      <c r="H9" t="s">
+        <v>167</v>
+      </c>
       <c r="I9" t="s">
         <v>46</v>
       </c>
@@ -1449,6 +1459,9 @@
       <c r="G10" t="s">
         <v>47</v>
       </c>
+      <c r="H10" t="s">
+        <v>167</v>
+      </c>
       <c r="I10" t="s">
         <v>49</v>
       </c>
@@ -1487,6 +1500,9 @@
       <c r="G11" t="s">
         <v>50</v>
       </c>
+      <c r="H11" t="s">
+        <v>167</v>
+      </c>
       <c r="I11" t="s">
         <v>147</v>
       </c>
@@ -1525,6 +1541,9 @@
       <c r="G12" t="s">
         <v>39</v>
       </c>
+      <c r="H12" t="s">
+        <v>167</v>
+      </c>
       <c r="I12" t="s">
         <v>53</v>
       </c>
@@ -1595,6 +1614,9 @@
       <c r="E15">
         <v>2000</v>
       </c>
+      <c r="H15" t="s">
+        <v>167</v>
+      </c>
       <c r="M15" t="s">
         <v>55</v>
       </c>
@@ -1618,6 +1640,9 @@
       <c r="E16">
         <v>2000</v>
       </c>
+      <c r="H16" t="s">
+        <v>167</v>
+      </c>
       <c r="J16" t="s">
         <v>132</v>
       </c>
@@ -1644,6 +1669,9 @@
       <c r="E17">
         <v>4000</v>
       </c>
+      <c r="H17" t="s">
+        <v>167</v>
+      </c>
       <c r="I17" t="s">
         <v>57</v>
       </c>
@@ -1708,6 +1736,9 @@
       <c r="E19">
         <v>8000</v>
       </c>
+      <c r="H19" t="s">
+        <v>167</v>
+      </c>
       <c r="I19" t="s">
         <v>60</v>
       </c>
@@ -1733,6 +1764,9 @@
       </c>
       <c r="E20">
         <v>5000</v>
+      </c>
+      <c r="H20" t="s">
+        <v>167</v>
       </c>
       <c r="I20" t="s">
         <v>61</v>
@@ -1788,13 +1822,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CFB178-60C6-42BA-9A7C-03EB8A68EE9C}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1834,7 +1868,7 @@
         <v>3.5</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>1.5</v>
@@ -1857,7 +1891,7 @@
         <v>3.5</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -1880,7 +1914,7 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="F4">
         <v>17</v>
@@ -1903,7 +1937,7 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>18</v>
@@ -1949,7 +1983,7 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -1972,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="F8">
         <v>30</v>
@@ -1995,7 +2029,7 @@
         <v>5</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="F9">
         <v>27</v>
@@ -2018,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>10</v>

</xml_diff>

<commit_message>
Bug fix: Special Tower Attack
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\Storm The House\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A61E8-C6A6-4D41-9971-21BE0FF059CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDDB5C3-D488-4239-8873-5B29F65161AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="181">
   <si>
     <t>AMMO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1668,6 +1668,9 @@
       <c r="N15" t="s">
         <v>55</v>
       </c>
+      <c r="O15" t="s">
+        <v>161</v>
+      </c>
       <c r="S15" t="s">
         <v>56</v>
       </c>
@@ -1699,6 +1702,9 @@
       </c>
       <c r="N16" t="s">
         <v>156</v>
+      </c>
+      <c r="O16" t="s">
+        <v>161</v>
       </c>
       <c r="T16" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
Bug fix: Down attack
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\Storm The House\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDDB5C3-D488-4239-8873-5B29F65161AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B04B0AA-4F1E-4577-B9D1-0DE736168A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="182">
   <si>
     <t>AMMO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -684,6 +684,10 @@
   </si>
   <si>
     <t>50;50;300;2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOWNABLE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1071,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D884F8-0FD5-40CA-AEA1-09465B4050E8}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -1895,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CFB178-60C6-42BA-9A7C-03EB8A68EE9C}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1909,7 +1913,7 @@
     <col min="7" max="7" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1934,8 +1938,11 @@
       <c r="H1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1960,8 +1967,11 @@
       <c r="H2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1986,8 +1996,11 @@
       <c r="H3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -2012,8 +2025,11 @@
       <c r="H4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -2038,8 +2054,11 @@
       <c r="H5">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -2064,8 +2083,11 @@
       <c r="H6">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -2090,8 +2112,11 @@
       <c r="H7">
         <v>130</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -2116,8 +2141,11 @@
       <c r="H8">
         <v>180</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -2142,8 +2170,11 @@
       <c r="H9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -2167,6 +2198,9 @@
       </c>
       <c r="H10">
         <v>1000</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="5:5" x14ac:dyDescent="0.3">

</xml_diff>